<commit_message>
Test cases for doctor login and registration
</commit_message>
<xml_diff>
--- a/Health-care System Test Cases Writing/Doctor login.xlsx
+++ b/Health-care System Test Cases Writing/Doctor login.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQA and Cyber Security Course\TestCase Github\Test-Cases\Health-care System Test Cases Writing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43C5E23-1257-4B69-B92A-D102A192383C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D031997-13DE-4D33-AB21-02EFC5A55AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,9 +130,6 @@
     <t>Shah Mainur Rahman</t>
   </si>
   <si>
-    <t>Test Cases for Login Process</t>
-  </si>
-  <si>
     <t>Login with valid username and password</t>
   </si>
   <si>
@@ -212,6 +209,9 @@
   </si>
   <si>
     <t>http://localhost/Health-care-system/pindex.php</t>
+  </si>
+  <si>
+    <t>Test Cases for Doctor Login Process</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1274,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1317,13 +1317,13 @@
       </c>
       <c r="I1" s="39"/>
     </row>
-    <row r="2" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="2" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>10</v>
@@ -1445,26 +1445,26 @@
         <v>30</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="17" t="s">
         <v>49</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>50</v>
       </c>
       <c r="H7" s="18" t="s">
         <v>0</v>
       </c>
       <c r="I7" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -1474,10 +1474,10 @@
         <v>29</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
@@ -1488,13 +1488,13 @@
       <c r="A9" s="20"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
@@ -1505,13 +1505,13 @@
       <c r="A10" s="15"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="17"/>
@@ -1522,11 +1522,11 @@
       <c r="A11" s="15"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
@@ -1538,28 +1538,28 @@
         <v>31</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>28</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H12" s="18" t="s">
         <v>0</v>
       </c>
       <c r="I12" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -1569,10 +1569,10 @@
         <v>29</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="17"/>
@@ -1583,11 +1583,11 @@
       <c r="A14" s="20"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="28"/>
       <c r="E14" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="17"/>
@@ -1599,28 +1599,28 @@
         <v>32</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>28</v>
       </c>
       <c r="D15" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>58</v>
-      </c>
       <c r="G15" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H15" s="18" t="s">
         <v>0</v>
       </c>
       <c r="I15" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -1630,10 +1630,10 @@
         <v>29</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="17"/>
@@ -1644,11 +1644,11 @@
       <c r="A17" s="21"/>
       <c r="B17" s="17"/>
       <c r="C17" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="29"/>
       <c r="E17" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
@@ -1660,28 +1660,28 @@
         <v>33</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>28</v>
       </c>
       <c r="D18" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>58</v>
-      </c>
       <c r="G18" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H18" s="18" t="s">
         <v>0</v>
       </c>
       <c r="I18" s="37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -1691,10 +1691,10 @@
         <v>29</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
@@ -1705,11 +1705,11 @@
       <c r="A20" s="21"/>
       <c r="B20" s="17"/>
       <c r="C20" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="29"/>
       <c r="E20" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>

</xml_diff>

<commit_message>
Test case for doctor Registration and login
</commit_message>
<xml_diff>
--- a/Health-care System Test Cases Writing/Doctor login.xlsx
+++ b/Health-care System Test Cases Writing/Doctor login.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQA and Cyber Security Course\TestCase Github\Test-Cases\Health-care System Test Cases Writing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D031997-13DE-4D33-AB21-02EFC5A55AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB85CC7-CD28-4142-889F-EC832FCA0C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25605" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="3" r:id="rId1"/>
@@ -208,10 +208,10 @@
     <t>InvalidUserNameAndValidPassword</t>
   </si>
   <si>
-    <t>http://localhost/Health-care-system/pindex.php</t>
-  </si>
-  <si>
     <t>Test Cases for Doctor Login Process</t>
+  </si>
+  <si>
+    <t>http://localhost/Health-care-system/index.php</t>
   </si>
 </sst>
 </file>
@@ -1272,9 +1272,9 @@
   </sheetPr>
   <dimension ref="A1:I981"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>10</v>
@@ -1474,7 +1474,7 @@
         <v>29</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>41</v>
@@ -3008,9 +3008,8 @@
     <hyperlink ref="I15" r:id="rId2" xr:uid="{1C25A5EB-8960-44C3-85E0-FFBEEA3918F1}"/>
     <hyperlink ref="I12" r:id="rId3" xr:uid="{A92349BB-70EE-43E8-8261-38211EFCE652}"/>
     <hyperlink ref="I18" r:id="rId4" xr:uid="{E6376FE9-A1F2-4465-8609-0EC7CAE0A8C5}"/>
-    <hyperlink ref="D8" r:id="rId5" xr:uid="{62363B88-6D3C-4249-A1B9-8131D04AC3B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId6"/>
+  <pageSetup orientation="landscape" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>